<commit_message>
Fixing errors discovered through linear model outlier test.
</commit_message>
<xml_diff>
--- a/Data/phenotypic data/RawData/2011 Data/BogUpper5-R8.xlsx
+++ b/Data/phenotypic data/RawData/2011 Data/BogUpper5-R8.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="100" windowWidth="25440" windowHeight="18140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1553,20 +1553,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1903,8 +1903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W811"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A793" workbookViewId="0">
-      <selection activeCell="V812" sqref="V812"/>
+    <sheetView tabSelected="1" topLeftCell="A543" workbookViewId="0">
+      <selection activeCell="M561" sqref="M561"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1964,52 +1964,52 @@
       <c r="T2" s="16"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="63" t="s">
         <v>256</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="63" t="s">
         <v>257</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
-      <c r="O4" s="65"/>
-      <c r="P4" s="65"/>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="65"/>
-      <c r="S4" s="65"/>
-      <c r="T4" s="65"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="63"/>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="4" t="s">
@@ -2130,28 +2130,28 @@
       <c r="T9" s="16"/>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="62" t="s">
         <v>262</v>
       </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="64"/>
-      <c r="N10" s="64"/>
-      <c r="O10" s="64"/>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="64"/>
-      <c r="R10" s="64"/>
-      <c r="S10" s="64"/>
-      <c r="T10" s="64"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="62"/>
+      <c r="O10" s="62"/>
+      <c r="P10" s="62"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="62"/>
+      <c r="T10" s="62"/>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="51"/>
@@ -2370,76 +2370,76 @@
       <c r="T19" s="5"/>
     </row>
     <row r="20" spans="1:22">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="62" t="s">
         <v>271</v>
       </c>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="64"/>
-      <c r="M20" s="64"/>
-      <c r="N20" s="64"/>
-      <c r="O20" s="64"/>
-      <c r="P20" s="64"/>
-      <c r="Q20" s="64"/>
-      <c r="R20" s="64"/>
-      <c r="S20" s="64"/>
-      <c r="T20" s="64"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="62"/>
+      <c r="N20" s="62"/>
+      <c r="O20" s="62"/>
+      <c r="P20" s="62"/>
+      <c r="Q20" s="62"/>
+      <c r="R20" s="62"/>
+      <c r="S20" s="62"/>
+      <c r="T20" s="62"/>
     </row>
     <row r="21" spans="1:22">
-      <c r="A21" s="64" t="s">
+      <c r="A21" s="62" t="s">
         <v>272</v>
       </c>
-      <c r="B21" s="64"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
-      <c r="K21" s="64"/>
-      <c r="L21" s="64"/>
-      <c r="M21" s="64"/>
-      <c r="N21" s="64"/>
-      <c r="O21" s="64"/>
-      <c r="P21" s="64"/>
-      <c r="Q21" s="64"/>
-      <c r="R21" s="64"/>
-      <c r="S21" s="64"/>
-      <c r="T21" s="64"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="62"/>
+      <c r="K21" s="62"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="62"/>
+      <c r="N21" s="62"/>
+      <c r="O21" s="62"/>
+      <c r="P21" s="62"/>
+      <c r="Q21" s="62"/>
+      <c r="R21" s="62"/>
+      <c r="S21" s="62"/>
+      <c r="T21" s="62"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="64" t="s">
+      <c r="A22" s="62" t="s">
         <v>273</v>
       </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="64"/>
-      <c r="L22" s="64"/>
-      <c r="M22" s="64"/>
-      <c r="N22" s="64"/>
-      <c r="O22" s="64"/>
-      <c r="P22" s="64"/>
-      <c r="Q22" s="64"/>
-      <c r="R22" s="64"/>
-      <c r="S22" s="64"/>
-      <c r="T22" s="64"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="62"/>
+      <c r="K22" s="62"/>
+      <c r="L22" s="62"/>
+      <c r="M22" s="62"/>
+      <c r="N22" s="62"/>
+      <c r="O22" s="62"/>
+      <c r="P22" s="62"/>
+      <c r="Q22" s="62"/>
+      <c r="R22" s="62"/>
+      <c r="S22" s="62"/>
+      <c r="T22" s="62"/>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="4"/>
@@ -2582,10 +2582,10 @@
       <c r="L31" s="20"/>
       <c r="M31" s="16"/>
       <c r="N31" s="41"/>
-      <c r="O31" s="63" t="s">
-        <v>3</v>
-      </c>
-      <c r="P31" s="63"/>
+      <c r="O31" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="P31" s="65"/>
       <c r="Q31" s="6"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
@@ -2606,11 +2606,11 @@
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="23"/>
-      <c r="K32" s="62" t="s">
+      <c r="K32" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="L32" s="62"/>
-      <c r="M32" s="62"/>
+      <c r="L32" s="64"/>
+      <c r="M32" s="64"/>
       <c r="N32" s="44" t="s">
         <v>6</v>
       </c>
@@ -4248,10 +4248,10 @@
       <c r="L60" s="20"/>
       <c r="M60" s="16"/>
       <c r="N60" s="41"/>
-      <c r="O60" s="63" t="s">
-        <v>3</v>
-      </c>
-      <c r="P60" s="63"/>
+      <c r="O60" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="P60" s="65"/>
       <c r="Q60" s="6"/>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
@@ -4272,11 +4272,11 @@
       </c>
       <c r="I61" s="1"/>
       <c r="J61" s="23"/>
-      <c r="K61" s="62" t="s">
+      <c r="K61" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="L61" s="62"/>
-      <c r="M61" s="62"/>
+      <c r="L61" s="64"/>
+      <c r="M61" s="64"/>
       <c r="N61" s="44" t="s">
         <v>6</v>
       </c>
@@ -5914,10 +5914,10 @@
       <c r="L89" s="20"/>
       <c r="M89" s="16"/>
       <c r="N89" s="41"/>
-      <c r="O89" s="63" t="s">
-        <v>3</v>
-      </c>
-      <c r="P89" s="63"/>
+      <c r="O89" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="P89" s="65"/>
       <c r="Q89" s="6"/>
       <c r="R89" s="1"/>
       <c r="S89" s="1"/>
@@ -5938,11 +5938,11 @@
       </c>
       <c r="I90" s="1"/>
       <c r="J90" s="23"/>
-      <c r="K90" s="62" t="s">
+      <c r="K90" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="L90" s="62"/>
-      <c r="M90" s="62"/>
+      <c r="L90" s="64"/>
+      <c r="M90" s="64"/>
       <c r="N90" s="44" t="s">
         <v>6</v>
       </c>
@@ -32410,7 +32410,7 @@
         <v>18.59</v>
       </c>
       <c r="M558" s="4">
-        <v>27.8</v>
+        <v>2.78</v>
       </c>
       <c r="N558" s="4">
         <v>3.58</v>
@@ -46828,18 +46828,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="K90:M90"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="O60:P60"/>
+    <mergeCell ref="K61:M61"/>
+    <mergeCell ref="O89:P89"/>
     <mergeCell ref="A22:T22"/>
     <mergeCell ref="A4:T4"/>
     <mergeCell ref="A3:T3"/>
     <mergeCell ref="A20:T20"/>
     <mergeCell ref="A21:T21"/>
     <mergeCell ref="A10:T10"/>
-    <mergeCell ref="K90:M90"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="K32:M32"/>
-    <mergeCell ref="O60:P60"/>
-    <mergeCell ref="K61:M61"/>
-    <mergeCell ref="O89:P89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>